<commit_message>
added a feature that fills in the DCF for you based on currecnt share price
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzafahad/Desktop/csc299-project-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D28C2-2DEF-C749-9CE1-D79EE9BEEB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498C30F3-DF31-094A-B285-3E219E35F9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2037,8 +2037,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="99" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2612,11 +2612,26 @@
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="45"/>
+      <c r="M12" s="44">
+        <f>M8+M10</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="44">
+        <f>N8+N10</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="44">
+        <f>O8+O10</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="44">
+        <f>P8+P10</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="45">
+        <f>Q8+Q10</f>
+        <v>0</v>
+      </c>
       <c r="R12" s="16"/>
       <c r="S12" s="1" t="s">
         <v>36</v>

</xml_diff>